<commit_message>
Did a bunch of tests with different models, results stored in LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
+++ b/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB49D3A-4E47-4462-BC4F-432366D0E58C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E88888F-D26A-4C70-9ADD-13B10D3B3F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="65">
   <si>
     <t>Model</t>
   </si>
@@ -168,13 +168,70 @@
   </si>
   <si>
     <t>RainBefore</t>
+  </si>
+  <si>
+    <t>OLS w/VIF Drop</t>
+  </si>
+  <si>
+    <t>OLS with variables dropped based on VIF scores</t>
+  </si>
+  <si>
+    <t>Thesis w/VIF Drop</t>
+  </si>
+  <si>
+    <t>T3 w/VIF Drop</t>
+  </si>
+  <si>
+    <t>Thesis /VIF Drop</t>
+  </si>
+  <si>
+    <t>T3 with variables dropped based on VIF scores</t>
+  </si>
+  <si>
+    <t>Thesis model with variables dropped based on VIF scores</t>
+  </si>
+  <si>
+    <t>T3 Variables</t>
+  </si>
+  <si>
+    <t>Current Best</t>
+  </si>
+  <si>
+    <t>OLS No Agg Weather</t>
+  </si>
+  <si>
+    <t>OLS No Specific Weather</t>
+  </si>
+  <si>
+    <t>T3 w/ Agg Weather</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T3 with the aggregated weather variables added back in</t>
+  </si>
+  <si>
+    <t>OLS with aggregated weather variables removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLS with specific weather variables removed </t>
+  </si>
+  <si>
+    <t>T3 based, with additional vars removed based on VIF and p-value</t>
+  </si>
+  <si>
+    <t>T7 v2</t>
+  </si>
+  <si>
+    <t>T7 based, with only weather variables being Clear and RainBefore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,8 +366,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,8 +587,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0066FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9966FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -680,6 +801,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -725,7 +868,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -744,22 +887,139 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="42" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="43" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -807,6 +1067,18 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FF9966FF"/>
+      <color rgb="FF0066FF"/>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FF00FFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1115,28 +1387,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1158,477 +1439,1423 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" s="85" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7">
+        <v>59</v>
+      </c>
+      <c r="C2" s="7">
+        <v>30</v>
+      </c>
+      <c r="D2" s="7">
+        <v>3641</v>
+      </c>
+      <c r="E2" s="7">
+        <v>721</v>
+      </c>
+      <c r="F2" s="7">
+        <v>66.72</v>
+      </c>
+      <c r="G2" s="7">
+        <v>83.43</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="84" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="25">
+        <v>58.612903225806448</v>
+      </c>
+      <c r="C3" s="25">
+        <v>29.93548387096774</v>
+      </c>
+      <c r="D3" s="25">
+        <v>3648.1290322580644</v>
+      </c>
+      <c r="E3" s="25">
+        <v>715.70967741935488</v>
+      </c>
+      <c r="F3" s="26">
+        <v>66.231651161750179</v>
+      </c>
+      <c r="G3" s="26">
+        <v>83.599978556178513</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="V3" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="84" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="70">
+        <v>58.612903225806448</v>
+      </c>
+      <c r="C4" s="70">
+        <v>29.93548387096774</v>
+      </c>
+      <c r="D4" s="70">
+        <v>3651.2580645161293</v>
+      </c>
+      <c r="E4" s="70">
+        <v>712.58064516129036</v>
+      </c>
+      <c r="F4" s="71">
+        <v>66.234574115930428</v>
+      </c>
+      <c r="G4" s="71">
+        <v>83.670863459810391</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="W4" s="84" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="79">
+        <v>57.741935483870968</v>
+      </c>
+      <c r="C5" s="79">
+        <v>30.806451612903224</v>
+      </c>
+      <c r="D5" s="79">
+        <v>3671.0645161290322</v>
+      </c>
+      <c r="E5" s="79">
+        <v>692.77419354838707</v>
+      </c>
+      <c r="F5" s="80">
+        <v>65.248387725679947</v>
+      </c>
+      <c r="G5" s="80">
+        <v>84.124666804865385</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="V5" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="89">
+        <v>57.548387096774192</v>
+      </c>
+      <c r="C6" s="89">
+        <v>31</v>
+      </c>
+      <c r="D6" s="89">
+        <v>3680.483870967742</v>
+      </c>
+      <c r="E6" s="89">
+        <v>683.35483870967744</v>
+      </c>
+      <c r="F6" s="90">
+        <v>64.979080829213643</v>
+      </c>
+      <c r="G6" s="90">
+        <v>84.339308846471425</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="U6" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="W6" s="84" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="32">
+        <v>58.387096774193552</v>
+      </c>
+      <c r="C7" s="32">
+        <v>30.161290322580644</v>
+      </c>
+      <c r="D7" s="32">
+        <v>3643.8387096774195</v>
+      </c>
+      <c r="E7" s="32">
+        <v>720</v>
+      </c>
+      <c r="F7" s="33">
+        <v>65.966205960882803</v>
+      </c>
+      <c r="G7" s="33">
+        <v>83.5018913340908</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="U7" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="V7" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="W7" s="84" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="B8" s="3">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3749</v>
+      </c>
+      <c r="E8" s="3">
+        <v>614</v>
+      </c>
+      <c r="F8" s="3">
+        <v>53.88</v>
+      </c>
+      <c r="G8" s="3">
+        <v>85.96</v>
+      </c>
+      <c r="J8" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="T8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="V8" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="W8" s="86" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18">
+        <v>57.548387096774192</v>
+      </c>
+      <c r="C9" s="18">
+        <v>31</v>
+      </c>
+      <c r="D9" s="18">
+        <v>3690.9032258064517</v>
+      </c>
+      <c r="E9" s="18">
+        <v>672.93548387096769</v>
+      </c>
+      <c r="F9" s="10">
+        <v>64.890597828680242</v>
+      </c>
+      <c r="G9" s="10">
+        <v>84.580813641304928</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="T9" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="U9" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="W9" s="84" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="21">
+        <v>47.70967741935484</v>
+      </c>
+      <c r="C10" s="21">
+        <v>40.838709677419352</v>
+      </c>
+      <c r="D10" s="21">
+        <v>3722.5806451612902</v>
+      </c>
+      <c r="E10" s="21">
+        <v>641.25806451612902</v>
+      </c>
+      <c r="F10" s="22">
+        <v>54.925524644539941</v>
+      </c>
+      <c r="G10" s="22">
+        <v>85.316371139179736</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="W10" s="84" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="B11" s="5">
+        <v>47</v>
+      </c>
+      <c r="C11" s="5">
+        <v>42</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3744</v>
+      </c>
+      <c r="E11" s="5">
+        <v>618</v>
+      </c>
+      <c r="F11" s="5">
+        <v>54.23</v>
+      </c>
+      <c r="G11" s="5">
+        <v>85.85</v>
+      </c>
+      <c r="J11" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="T11" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="U11" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="V11" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="W11" s="34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="62">
+        <v>46.258064516129032</v>
+      </c>
+      <c r="C12" s="62">
+        <v>42.29032258064516</v>
+      </c>
+      <c r="D12" s="62">
+        <v>3826.9677419354839</v>
+      </c>
+      <c r="E12" s="62">
+        <v>536.87096774193549</v>
+      </c>
+      <c r="F12" s="63">
+        <v>52.787579755345718</v>
+      </c>
+      <c r="G12" s="63">
+        <v>87.721533344561493</v>
+      </c>
+      <c r="J12" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="S12" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="T12" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="U12" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="V12" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="W12" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="66">
+        <v>57.41935483870968</v>
+      </c>
+      <c r="C13" s="66">
+        <v>31.129032258064516</v>
+      </c>
+      <c r="D13" s="66">
+        <v>3692.0967741935483</v>
+      </c>
+      <c r="E13" s="66">
+        <v>671.74193548387098</v>
+      </c>
+      <c r="F13" s="67">
+        <v>64.817892699130013</v>
+      </c>
+      <c r="G13" s="67">
+        <v>84.607038002688725</v>
+      </c>
+      <c r="J13" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="T13" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="U13" s="81" t="s">
+        <v>24</v>
+      </c>
+      <c r="V13" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J14" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="V14" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="W14" s="34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J15" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="O15" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U15" s="81" t="s">
+        <v>28</v>
+      </c>
+      <c r="V15" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="W15" s="34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J16" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="U16" s="81" t="s">
+        <v>29</v>
+      </c>
+      <c r="V16" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="W16" s="34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J17" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U17" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="V17" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="W17" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J18" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U18" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="V18" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="W18" s="34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J19" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="N19" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U19" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="V19" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="W19" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J20" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="O20" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="P21" s="34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="O22" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="P22" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="B23" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="L26" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="O26" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="P26" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="O27" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="P27" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3">
-        <v>3749</v>
-      </c>
-      <c r="E2" s="3">
-        <v>614</v>
-      </c>
-      <c r="F2" s="3">
-        <v>53.88</v>
-      </c>
-      <c r="G2" s="3">
-        <v>85.96</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5">
-        <v>47</v>
-      </c>
-      <c r="C3" s="5">
-        <v>42</v>
-      </c>
-      <c r="D3" s="5">
-        <v>3744</v>
-      </c>
-      <c r="E3" s="5">
-        <v>618</v>
-      </c>
-      <c r="F3" s="5">
-        <v>54.23</v>
-      </c>
-      <c r="G3" s="5">
-        <v>85.85</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="7">
-        <v>59</v>
-      </c>
-      <c r="C4" s="7">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7">
-        <v>3641</v>
-      </c>
-      <c r="E4" s="7">
-        <v>721</v>
-      </c>
-      <c r="F4" s="7">
-        <v>66.72</v>
-      </c>
-      <c r="G4" s="7">
-        <v>83.43</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="23">
-        <v>57.548387096774192</v>
-      </c>
-      <c r="C5" s="23">
-        <v>31</v>
-      </c>
-      <c r="D5" s="23">
-        <v>3690.9032258064517</v>
-      </c>
-      <c r="E5" s="23">
-        <v>672.93548387096769</v>
-      </c>
-      <c r="F5" s="10">
-        <v>64.890597828680242</v>
-      </c>
-      <c r="G5" s="10">
-        <v>84.580813641304928</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" s="13" t="s">
+      <c r="M28" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="13"/>
-      <c r="M13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="13"/>
-      <c r="M15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="N28" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="O28" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="75"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="87"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="J16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="13"/>
-      <c r="M16" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="13"/>
-      <c r="M17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="13"/>
-      <c r="M18" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J19" s="3"/>
-      <c r="K19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J20" s="3"/>
-      <c r="K20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L20" s="13"/>
-      <c r="M20" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="M21" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="M22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="M23" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="M24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="M25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="M26" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="M27" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="M28" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="A16:H16"/>
+  <mergeCells count="13">
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B32:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Doing some additional variable tests
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
+++ b/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E88888F-D26A-4C70-9ADD-13B10D3B3F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DAE460-35F3-4E23-A039-9C1D65F944C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="67">
   <si>
     <t>Model</t>
   </si>
@@ -225,12 +225,21 @@
   </si>
   <si>
     <t>T7 based, with only weather variables being Clear and RainBefore</t>
+  </si>
+  <si>
+    <t>T7 v3</t>
+  </si>
+  <si>
+    <t>Altered version of T7, with vars dropped based on VIF and p-value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,7 +392,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="45">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +641,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,7 +883,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -887,21 +902,17 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -909,102 +920,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="42" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="43" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1014,12 +943,107 @@
     <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="45" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="45" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="45" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1069,6 +1093,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCC00"/>
       <color rgb="FFCCCCFF"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FF9966FF"/>
@@ -1387,18 +1412,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -1415,9 +1440,10 @@
     <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1439,19 +1465,19 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="32" t="s">
         <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="61" t="s">
+      <c r="N1" s="35" t="s">
         <v>56</v>
       </c>
       <c r="O1" s="8" t="s">
@@ -1460,42 +1486,45 @@
       <c r="P1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="32" t="s">
         <v>53</v>
       </c>
       <c r="R1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="S1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="T1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="68" t="s">
+      <c r="U1" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="78" t="s">
+      <c r="V1" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="85" t="s">
+      <c r="W1" s="51" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="92" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="80">
         <v>59</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="80">
         <v>30</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="80">
         <v>3641</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="80">
         <v>721</v>
       </c>
       <c r="F2" s="7">
@@ -1504,19 +1533,19 @@
       <c r="G2" s="7">
         <v>83.43</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="32" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="60" t="s">
+      <c r="M2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="61" t="s">
+      <c r="N2" s="35" t="s">
         <v>10</v>
       </c>
       <c r="O2" s="9" t="s">
@@ -1525,63 +1554,66 @@
       <c r="P2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="36" t="s">
+      <c r="Q2" s="32" t="s">
         <v>10</v>
       </c>
       <c r="R2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="S2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="69" t="s">
+      <c r="U2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="76" t="s">
+      <c r="V2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="50" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="X2" s="93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="81">
         <v>58.612903225806448</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="81">
         <v>29.93548387096774</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="81">
         <v>3648.1290322580644</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="81">
         <v>715.70967741935488</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="23">
         <v>66.231651161750179</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="23">
         <v>83.599978556178513</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="32" t="s">
         <v>11</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="61" t="s">
+      <c r="N3" s="35" t="s">
         <v>11</v>
       </c>
       <c r="O3" s="9" t="s">
@@ -1590,63 +1622,66 @@
       <c r="P3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="Q3" s="32" t="s">
         <v>11</v>
       </c>
       <c r="R3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="S3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="31" t="s">
+      <c r="T3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="69" t="s">
+      <c r="U3" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="76" t="s">
+      <c r="V3" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="84" t="s">
+      <c r="W3" s="50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
+      <c r="X3" s="93" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="70">
+      <c r="B4" s="82">
         <v>58.612903225806448</v>
       </c>
-      <c r="C4" s="70">
+      <c r="C4" s="82">
         <v>29.93548387096774</v>
       </c>
-      <c r="D4" s="70">
+      <c r="D4" s="82">
         <v>3651.2580645161293</v>
       </c>
-      <c r="E4" s="70">
+      <c r="E4" s="82">
         <v>712.58064516129036</v>
       </c>
-      <c r="F4" s="71">
+      <c r="F4" s="42">
         <v>66.234574115930428</v>
       </c>
-      <c r="G4" s="71">
+      <c r="G4" s="42">
         <v>83.670863459810391</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="32" t="s">
         <v>12</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="60" t="s">
+      <c r="M4" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="61" t="s">
+      <c r="N4" s="35" t="s">
         <v>12</v>
       </c>
       <c r="O4" s="9" t="s">
@@ -1655,63 +1690,66 @@
       <c r="P4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="36" t="s">
+      <c r="Q4" s="32" t="s">
         <v>12</v>
       </c>
       <c r="R4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="31" t="s">
+      <c r="T4" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="U4" s="69" t="s">
+      <c r="U4" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="V4" s="76" t="s">
+      <c r="V4" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="W4" s="84" t="s">
+      <c r="W4" s="50" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
+      <c r="X4" s="93" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="83">
         <v>57.741935483870968</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="83">
         <v>30.806451612903224</v>
       </c>
-      <c r="D5" s="79">
+      <c r="D5" s="83">
         <v>3671.0645161290322</v>
       </c>
-      <c r="E5" s="79">
+      <c r="E5" s="83">
         <v>692.77419354838707</v>
       </c>
-      <c r="F5" s="80">
+      <c r="F5" s="46">
         <v>65.248387725679947</v>
       </c>
-      <c r="G5" s="80">
+      <c r="G5" s="46">
         <v>84.124666804865385</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="32" t="s">
         <v>31</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="60" t="s">
+      <c r="M5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="61" t="s">
+      <c r="N5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="O5" s="9" t="s">
@@ -1720,66 +1758,69 @@
       <c r="P5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="36" t="s">
+      <c r="Q5" s="32" t="s">
         <v>31</v>
       </c>
       <c r="R5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="S5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="T5" s="31" t="s">
+      <c r="T5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="69" t="s">
+      <c r="U5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="V5" s="76" t="s">
+      <c r="V5" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="W5" s="84" t="s">
+      <c r="W5" s="50" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="85" t="s">
+      <c r="X5" s="93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="89">
+      <c r="B6" s="84">
         <v>57.548387096774192</v>
       </c>
-      <c r="C6" s="89">
+      <c r="C6" s="84">
         <v>31</v>
       </c>
-      <c r="D6" s="89">
+      <c r="D6" s="84">
         <v>3680.483870967742</v>
       </c>
-      <c r="E6" s="89">
+      <c r="E6" s="84">
         <v>683.35483870967744</v>
       </c>
-      <c r="F6" s="90">
+      <c r="F6" s="53">
         <v>64.979080829213643</v>
       </c>
-      <c r="G6" s="90">
+      <c r="G6" s="53">
         <v>84.339308846471425</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="32" t="s">
         <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="60" t="s">
+      <c r="M6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="61" t="s">
+      <c r="N6" s="35" t="s">
         <v>14</v>
       </c>
       <c r="O6" s="9" t="s">
@@ -1788,63 +1829,66 @@
       <c r="P6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="36" t="s">
+      <c r="Q6" s="32" t="s">
         <v>13</v>
       </c>
       <c r="R6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="24" t="s">
+      <c r="S6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="T6" s="31" t="s">
+      <c r="T6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="U6" s="69" t="s">
+      <c r="U6" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="V6" s="76" t="s">
+      <c r="V6" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="W6" s="84" t="s">
+      <c r="W6" s="50" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="32">
-        <v>58.387096774193552</v>
-      </c>
-      <c r="C7" s="32">
-        <v>30.161290322580644</v>
-      </c>
-      <c r="D7" s="32">
-        <v>3643.8387096774195</v>
-      </c>
-      <c r="E7" s="32">
-        <v>720</v>
-      </c>
-      <c r="F7" s="33">
-        <v>65.966205960882803</v>
-      </c>
-      <c r="G7" s="33">
-        <v>83.5018913340908</v>
-      </c>
-      <c r="J7" s="36" t="s">
+      <c r="X6" s="93" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="92" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="94">
+        <v>57.935483870967744</v>
+      </c>
+      <c r="C7" s="94">
+        <v>30.612903225806452</v>
+      </c>
+      <c r="D7" s="94">
+        <v>3667.0645161290322</v>
+      </c>
+      <c r="E7" s="94">
+        <v>696.77419354838707</v>
+      </c>
+      <c r="F7" s="95">
+        <v>65.47266280686857</v>
+      </c>
+      <c r="G7" s="95">
+        <v>84.03324265116818</v>
+      </c>
+      <c r="J7" s="32" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="60" t="s">
+      <c r="M7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="61" t="s">
+      <c r="N7" s="35" t="s">
         <v>15</v>
       </c>
       <c r="O7" s="9" t="s">
@@ -1853,997 +1897,1072 @@
       <c r="P7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q7" s="36" t="s">
+      <c r="Q7" s="32" t="s">
         <v>14</v>
       </c>
       <c r="R7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S7" s="24" t="s">
+      <c r="S7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="T7" s="31" t="s">
+      <c r="T7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="U7" s="69" t="s">
+      <c r="U7" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="V7" s="76" t="s">
+      <c r="V7" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="W7" s="84" t="s">
+      <c r="W7" s="50" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3">
-        <v>47</v>
-      </c>
-      <c r="C8" s="3">
-        <v>42</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3749</v>
-      </c>
-      <c r="E8" s="3">
-        <v>614</v>
-      </c>
-      <c r="F8" s="3">
-        <v>53.88</v>
-      </c>
-      <c r="G8" s="3">
-        <v>85.96</v>
-      </c>
-      <c r="J8" s="36" t="s">
+      <c r="X7" s="93" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="85">
+        <v>58.387096774193552</v>
+      </c>
+      <c r="C8" s="85">
+        <v>30.161290322580644</v>
+      </c>
+      <c r="D8" s="85">
+        <v>3643.8387096774195</v>
+      </c>
+      <c r="E8" s="85">
+        <v>720</v>
+      </c>
+      <c r="F8" s="29">
+        <v>65.966205960882803</v>
+      </c>
+      <c r="G8" s="29">
+        <v>83.5018913340908</v>
+      </c>
+      <c r="J8" s="32" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="60" t="s">
+      <c r="M8" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="61" t="s">
+      <c r="N8" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="30" t="s">
         <v>12</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="36" t="s">
+      <c r="Q8" s="32" t="s">
         <v>32</v>
       </c>
       <c r="R8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="S8" s="24" t="s">
+      <c r="S8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="T8" s="31" t="s">
+      <c r="T8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="U8" s="69" t="s">
+      <c r="U8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="V8" s="83" t="s">
+      <c r="V8" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="W8" s="86" t="s">
+      <c r="W8" s="52" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="18">
-        <v>57.548387096774192</v>
-      </c>
-      <c r="C9" s="18">
-        <v>31</v>
-      </c>
-      <c r="D9" s="18">
-        <v>3690.9032258064517</v>
-      </c>
-      <c r="E9" s="18">
-        <v>672.93548387096769</v>
-      </c>
-      <c r="F9" s="10">
-        <v>64.890597828680242</v>
-      </c>
-      <c r="G9" s="10">
-        <v>84.580813641304928</v>
-      </c>
-      <c r="J9" s="36" t="s">
+      <c r="X8" s="93" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="86">
+        <v>47</v>
+      </c>
+      <c r="C9" s="86">
+        <v>42</v>
+      </c>
+      <c r="D9" s="86">
+        <v>3749</v>
+      </c>
+      <c r="E9" s="86">
+        <v>614</v>
+      </c>
+      <c r="F9" s="3">
+        <v>53.88</v>
+      </c>
+      <c r="G9" s="3">
+        <v>85.96</v>
+      </c>
+      <c r="J9" s="32" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="L9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="60" t="s">
+      <c r="M9" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="61" t="s">
+      <c r="N9" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="O9" s="30" t="s">
         <v>16</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="36" t="s">
+      <c r="Q9" s="32" t="s">
         <v>15</v>
       </c>
       <c r="R9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="S9" s="24" t="s">
+      <c r="S9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="T9" s="31" t="s">
+      <c r="T9" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="U9" s="69" t="s">
+      <c r="U9" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="76" t="s">
+      <c r="V9" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="W9" s="84" t="s">
+      <c r="W9" s="50" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="21">
-        <v>47.70967741935484</v>
-      </c>
-      <c r="C10" s="21">
-        <v>40.838709677419352</v>
-      </c>
-      <c r="D10" s="21">
-        <v>3722.5806451612902</v>
-      </c>
-      <c r="E10" s="21">
-        <v>641.25806451612902</v>
-      </c>
-      <c r="F10" s="22">
-        <v>54.925524644539941</v>
-      </c>
-      <c r="G10" s="22">
-        <v>85.316371139179736</v>
-      </c>
-      <c r="J10" s="36" t="s">
+      <c r="X9" s="93" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="87">
+        <v>57.548387096774192</v>
+      </c>
+      <c r="C10" s="87">
+        <v>31</v>
+      </c>
+      <c r="D10" s="87">
+        <v>3690.9032258064517</v>
+      </c>
+      <c r="E10" s="87">
+        <v>672.93548387096769</v>
+      </c>
+      <c r="F10" s="10">
+        <v>64.890597828680242</v>
+      </c>
+      <c r="G10" s="10">
+        <v>84.580813641304928</v>
+      </c>
+      <c r="J10" s="32" t="s">
         <v>27</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="20" t="s">
+      <c r="L10" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="60" t="s">
+      <c r="M10" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="61" t="s">
+      <c r="N10" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="34" t="s">
+      <c r="O10" s="30" t="s">
         <v>17</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="36" t="s">
+      <c r="Q10" s="32" t="s">
         <v>27</v>
       </c>
       <c r="R10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="S10" s="24" t="s">
+      <c r="S10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="T10" s="29" t="s">
+      <c r="T10" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="U10" s="69" t="s">
+      <c r="U10" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="V10" s="76" t="s">
+      <c r="V10" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="W10" s="84" t="s">
+      <c r="W10" s="30" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5">
-        <v>47</v>
-      </c>
-      <c r="C11" s="5">
-        <v>42</v>
-      </c>
-      <c r="D11" s="5">
-        <v>3744</v>
-      </c>
-      <c r="E11" s="5">
-        <v>618</v>
-      </c>
-      <c r="F11" s="5">
-        <v>54.23</v>
-      </c>
-      <c r="G11" s="5">
-        <v>85.85</v>
-      </c>
-      <c r="J11" s="36" t="s">
+      <c r="X10" s="93" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="88">
+        <v>47.70967741935484</v>
+      </c>
+      <c r="C11" s="88">
+        <v>40.838709677419352</v>
+      </c>
+      <c r="D11" s="88">
+        <v>3722.5806451612902</v>
+      </c>
+      <c r="E11" s="88">
+        <v>641.25806451612902</v>
+      </c>
+      <c r="F11" s="20">
+        <v>54.925524644539941</v>
+      </c>
+      <c r="G11" s="20">
+        <v>85.316371139179736</v>
+      </c>
+      <c r="J11" s="32" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="60" t="s">
+      <c r="M11" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="34" t="s">
+      <c r="N11" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="34" t="s">
+      <c r="O11" s="30" t="s">
         <v>18</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="36" t="s">
+      <c r="Q11" s="32" t="s">
         <v>26</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="S11" s="24" t="s">
+      <c r="S11" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="T11" s="34" t="s">
+      <c r="T11" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="U11" s="69" t="s">
+      <c r="U11" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="V11" s="76" t="s">
+      <c r="V11" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="W11" s="34" t="s">
+      <c r="W11" s="30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="62">
-        <v>46.258064516129032</v>
-      </c>
-      <c r="C12" s="62">
-        <v>42.29032258064516</v>
-      </c>
-      <c r="D12" s="62">
-        <v>3826.9677419354839</v>
-      </c>
-      <c r="E12" s="62">
-        <v>536.87096774193549</v>
-      </c>
-      <c r="F12" s="63">
-        <v>52.787579755345718</v>
-      </c>
-      <c r="G12" s="63">
-        <v>87.721533344561493</v>
-      </c>
-      <c r="J12" s="36" t="s">
+      <c r="X11" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="89">
+        <v>47</v>
+      </c>
+      <c r="C12" s="89">
+        <v>42</v>
+      </c>
+      <c r="D12" s="89">
+        <v>3744</v>
+      </c>
+      <c r="E12" s="89">
+        <v>618</v>
+      </c>
+      <c r="F12" s="5">
+        <v>54.23</v>
+      </c>
+      <c r="G12" s="5">
+        <v>85.85</v>
+      </c>
+      <c r="J12" s="32" t="s">
         <v>42</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="20" t="s">
+      <c r="L12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="60" t="s">
+      <c r="M12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="34" t="s">
+      <c r="N12" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="30" t="s">
         <v>19</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q12" s="36" t="s">
+      <c r="Q12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="R12" s="34" t="s">
+      <c r="R12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="S12" s="24" t="s">
+      <c r="S12" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="T12" s="34" t="s">
+      <c r="T12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="U12" s="69" t="s">
+      <c r="U12" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="V12" s="76" t="s">
+      <c r="V12" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="W12" s="34" t="s">
+      <c r="W12" s="30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="66">
-        <v>57.41935483870968</v>
-      </c>
-      <c r="C13" s="66">
-        <v>31.129032258064516</v>
-      </c>
-      <c r="D13" s="66">
-        <v>3692.0967741935483</v>
-      </c>
-      <c r="E13" s="66">
-        <v>671.74193548387098</v>
-      </c>
-      <c r="F13" s="67">
-        <v>64.817892699130013</v>
-      </c>
-      <c r="G13" s="67">
-        <v>84.607038002688725</v>
-      </c>
-      <c r="J13" s="36" t="s">
+      <c r="X12" s="30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="90">
+        <v>46.258064516129032</v>
+      </c>
+      <c r="C13" s="90">
+        <v>42.29032258064516</v>
+      </c>
+      <c r="D13" s="90">
+        <v>3826.9677419354839</v>
+      </c>
+      <c r="E13" s="90">
+        <v>536.87096774193549</v>
+      </c>
+      <c r="F13" s="36">
+        <v>52.787579755345718</v>
+      </c>
+      <c r="G13" s="36">
+        <v>87.721533344561493</v>
+      </c>
+      <c r="J13" s="32" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="20" t="s">
+      <c r="L13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="60" t="s">
+      <c r="M13" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="34" t="s">
+      <c r="N13" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="34" t="s">
+      <c r="O13" s="30" t="s">
         <v>20</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q13" s="36" t="s">
+      <c r="Q13" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="R13" s="34" t="s">
+      <c r="R13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="S13" s="34" t="s">
+      <c r="S13" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="T13" s="34" t="s">
+      <c r="T13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="U13" s="81" t="s">
+      <c r="U13" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="V13" s="76" t="s">
+      <c r="V13" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="W13" s="34" t="s">
+      <c r="W13" s="30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J14" s="36" t="s">
+      <c r="X13" s="30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="91">
+        <v>57.41935483870968</v>
+      </c>
+      <c r="C14" s="91">
+        <v>31.129032258064516</v>
+      </c>
+      <c r="D14" s="91">
+        <v>3692.0967741935483</v>
+      </c>
+      <c r="E14" s="91">
+        <v>671.74193548387098</v>
+      </c>
+      <c r="F14" s="39">
+        <v>64.817892699130013</v>
+      </c>
+      <c r="G14" s="39">
+        <v>84.607038002688725</v>
+      </c>
+      <c r="J14" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="20" t="s">
+      <c r="L14" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="60" t="s">
+      <c r="M14" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="34" t="s">
+      <c r="N14" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="34" t="s">
+      <c r="O14" s="30" t="s">
         <v>21</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="U14" s="81" t="s">
+      <c r="U14" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="V14" s="34" t="s">
+      <c r="V14" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="W14" s="34" t="s">
+      <c r="W14" s="30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J15" s="36" t="s">
+      <c r="X14" s="30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J15" s="32" t="s">
         <v>43</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="20" t="s">
+      <c r="L15" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="M15" s="60" t="s">
+      <c r="M15" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="34" t="s">
+      <c r="N15" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="34" t="s">
+      <c r="O15" s="30" t="s">
         <v>22</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="U15" s="81" t="s">
+      <c r="U15" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="V15" s="34" t="s">
+      <c r="V15" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="W15" s="34" t="s">
+      <c r="W15" s="30" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J16" s="36" t="s">
+      <c r="X15" s="30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J16" s="32" t="s">
         <v>44</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="20" t="s">
+      <c r="L16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="60" t="s">
+      <c r="M16" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="34" t="s">
+      <c r="N16" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="O16" s="34" t="s">
+      <c r="O16" s="30" t="s">
         <v>23</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="U16" s="81" t="s">
+      <c r="U16" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="V16" s="34" t="s">
+      <c r="V16" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="W16" s="34" t="s">
+      <c r="W16" s="30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J17" s="36" t="s">
+      <c r="X16" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J17" s="32" t="s">
         <v>21</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="34" t="s">
+      <c r="L17" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="34" t="s">
+      <c r="M17" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="N17" s="34" t="s">
+      <c r="N17" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="O17" s="34" t="s">
+      <c r="O17" s="30" t="s">
         <v>24</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="81" t="s">
+      <c r="U17" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="V17" s="34" t="s">
+      <c r="V17" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="W17" s="34" t="s">
+      <c r="W17" s="30" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J18" s="36" t="s">
+      <c r="X17" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J18" s="32" t="s">
         <v>22</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="34" t="s">
+      <c r="L18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="34" t="s">
+      <c r="M18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="O18" s="34" t="s">
+      <c r="O18" s="30" t="s">
         <v>25</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="U18" s="81" t="s">
+      <c r="U18" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="V18" s="34" t="s">
+      <c r="V18" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="W18" s="34" t="s">
+      <c r="W18" s="30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J19" s="36" t="s">
+      <c r="X18" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J19" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="34" t="s">
+      <c r="K19" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="34" t="s">
+      <c r="L19" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="M19" s="34" t="s">
+      <c r="M19" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="N19" s="34" t="s">
+      <c r="N19" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="O19" s="34" t="s">
+      <c r="O19" s="30" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="U19" s="82" t="s">
+      <c r="U19" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="V19" s="34" t="s">
+      <c r="V19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="W19" s="34" t="s">
+      <c r="W19" s="30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J20" s="36" t="s">
+      <c r="X19" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J20" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="35" t="s">
+      <c r="L20" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="M20" s="34" t="s">
+      <c r="M20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="N20" s="34" t="s">
+      <c r="N20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="O20" s="34" t="s">
+      <c r="O20" s="30" t="s">
         <v>32</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="36" t="s">
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="K21" s="34" t="s">
+      <c r="K21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="L21" s="34" t="s">
+      <c r="L21" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="M21" s="34" t="s">
+      <c r="M21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="N21" s="34" t="s">
+      <c r="N21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="O21" s="34" t="s">
+      <c r="O21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="P21" s="34" t="s">
+      <c r="P21" s="30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="36" t="s">
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="35" t="s">
+      <c r="K22" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="L22" s="34" t="s">
+      <c r="L22" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="M22" s="35" t="s">
+      <c r="M22" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N22" s="35" t="s">
+      <c r="N22" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O22" s="34" t="s">
+      <c r="O22" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="P22" s="34" t="s">
+      <c r="P22" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="36" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="34" t="s">
+      <c r="K23" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="34" t="s">
+      <c r="L23" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="M23" s="34" t="s">
+      <c r="M23" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="N23" s="34" t="s">
+      <c r="N23" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="O23" s="34" t="s">
+      <c r="O23" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="P23" s="34" t="s">
+      <c r="P23" s="30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="36" t="s">
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="34" t="s">
+      <c r="K24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="L24" s="34" t="s">
+      <c r="L24" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M24" s="34" t="s">
+      <c r="M24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="N24" s="34" t="s">
+      <c r="N24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="O24" s="34" t="s">
+      <c r="O24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="P24" s="34" t="s">
+      <c r="P24" s="30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="36" t="s">
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="K25" s="34" t="s">
+      <c r="K25" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="L25" s="34" t="s">
+      <c r="L25" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="N25" s="34" t="s">
+      <c r="N25" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="O25" s="34" t="s">
+      <c r="O25" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="P25" s="34" t="s">
+      <c r="P25" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="36" t="s">
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="34" t="s">
+      <c r="K26" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="L26" s="34" t="s">
+      <c r="L26" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="34" t="s">
+      <c r="M26" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="N26" s="34" t="s">
+      <c r="N26" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="O26" s="34" t="s">
+      <c r="O26" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="P26" s="34" t="s">
+      <c r="P26" s="30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="36" t="s">
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="69"/>
+      <c r="J27" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="34" t="s">
+      <c r="K27" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="34" t="s">
+      <c r="L27" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="M27" s="34" t="s">
+      <c r="M27" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="N27" s="34" t="s">
+      <c r="N27" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="O27" s="34" t="s">
+      <c r="O27" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="P27" s="34" t="s">
+      <c r="P27" s="30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="68" t="s">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="72" t="s">
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="34" t="s">
+      <c r="K28" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="L28" s="34" t="s">
+      <c r="L28" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="M28" s="34" t="s">
+      <c r="M28" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="N28" s="34" t="s">
+      <c r="N28" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="O28" s="34" t="s">
+      <c r="O28" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="P28" s="34" t="s">
+      <c r="P28" s="30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="64" t="s">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="74" t="s">
+      <c r="B29" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="65" t="s">
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="78" t="s">
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="77" t="s">
+      <c r="B31" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" s="88" t="s">
+      <c r="C31" s="79"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="87" t="s">
+      <c r="B32" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="87"/>
-      <c r="I32" s="87"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="92" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="96"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="96"/>
+      <c r="F33" s="96"/>
+      <c r="G33" s="96"/>
+      <c r="H33" s="96"/>
+      <c r="I33" s="96"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A33:I33"/>
+  <mergeCells count="14">
+    <mergeCell ref="A34:I34"/>
     <mergeCell ref="B22:I22"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B23:I23"/>
@@ -2856,6 +2975,7 @@
     <mergeCell ref="B28:I28"/>
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:I33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Doing some preliminary work for updating our dataset to have 2020 accidents.
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
+++ b/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DAE460-35F3-4E23-A039-9C1D65F944C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C53441E-4B06-4606-9193-806497BFCD17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="70">
   <si>
     <t>Model</t>
   </si>
@@ -231,15 +231,21 @@
   </si>
   <si>
     <t>Altered version of T7, with vars dropped based on VIF and p-value</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>Same as T7 v2, but with the added variable roundAbout</t>
+  </si>
+  <si>
+    <t>roundAbout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,7 +398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -647,6 +653,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF33"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -883,7 +895,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -944,6 +956,9 @@
     <xf numFmtId="0" fontId="16" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="45" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="45" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1022,28 +1037,40 @@
     <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="45" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="45" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="45" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="44" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="45" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="46" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="46" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="46" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1093,6 +1120,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFF33"/>
       <color rgb="FFFFCC00"/>
       <color rgb="FFCCCCFF"/>
       <color rgb="FFFF7C80"/>
@@ -1412,22 +1440,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -1441,9 +1470,10 @@
     <col min="21" max="21" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1507,24 +1537,27 @@
       <c r="W1" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="X1" s="92" t="s">
+      <c r="X1" s="54" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1" s="104" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="80">
+      <c r="B2" s="85">
         <v>59</v>
       </c>
-      <c r="C2" s="80">
+      <c r="C2" s="85">
         <v>30</v>
       </c>
-      <c r="D2" s="80">
+      <c r="D2" s="85">
         <v>3641</v>
       </c>
-      <c r="E2" s="80">
+      <c r="E2" s="85">
         <v>721</v>
       </c>
       <c r="F2" s="7">
@@ -1575,24 +1608,27 @@
       <c r="W2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="93" t="s">
+      <c r="X2" s="55" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2" s="98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="81">
+      <c r="B3" s="86">
         <v>58.612903225806448</v>
       </c>
-      <c r="C3" s="81">
+      <c r="C3" s="86">
         <v>29.93548387096774</v>
       </c>
-      <c r="D3" s="81">
+      <c r="D3" s="86">
         <v>3648.1290322580644</v>
       </c>
-      <c r="E3" s="81">
+      <c r="E3" s="86">
         <v>715.70967741935488</v>
       </c>
       <c r="F3" s="23">
@@ -1643,24 +1679,27 @@
       <c r="W3" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="X3" s="93" t="s">
+      <c r="X3" s="55" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3" s="98" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="82">
+      <c r="B4" s="87">
         <v>58.612903225806448</v>
       </c>
-      <c r="C4" s="82">
+      <c r="C4" s="87">
         <v>29.93548387096774</v>
       </c>
-      <c r="D4" s="82">
+      <c r="D4" s="87">
         <v>3651.2580645161293</v>
       </c>
-      <c r="E4" s="82">
+      <c r="E4" s="87">
         <v>712.58064516129036</v>
       </c>
       <c r="F4" s="42">
@@ -1711,24 +1750,27 @@
       <c r="W4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="93" t="s">
+      <c r="X4" s="55" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y4" s="98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="83">
+      <c r="B5" s="88">
         <v>57.741935483870968</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="88">
         <v>30.806451612903224</v>
       </c>
-      <c r="D5" s="83">
+      <c r="D5" s="88">
         <v>3671.0645161290322</v>
       </c>
-      <c r="E5" s="83">
+      <c r="E5" s="88">
         <v>692.77419354838707</v>
       </c>
       <c r="F5" s="46">
@@ -1779,24 +1821,27 @@
       <c r="W5" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="93" t="s">
+      <c r="X5" s="55" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5" s="98" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="84">
+      <c r="B6" s="89">
         <v>57.548387096774192</v>
       </c>
-      <c r="C6" s="84">
+      <c r="C6" s="89">
         <v>31</v>
       </c>
-      <c r="D6" s="84">
+      <c r="D6" s="89">
         <v>3680.483870967742</v>
       </c>
-      <c r="E6" s="84">
+      <c r="E6" s="89">
         <v>683.35483870967744</v>
       </c>
       <c r="F6" s="53">
@@ -1850,31 +1895,34 @@
       <c r="W6" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="X6" s="93" t="s">
+      <c r="X6" s="55" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="92" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="94">
-        <v>57.935483870967744</v>
-      </c>
-      <c r="C7" s="94">
-        <v>30.612903225806452</v>
-      </c>
-      <c r="D7" s="94">
-        <v>3667.0645161290322</v>
-      </c>
-      <c r="E7" s="94">
-        <v>696.77419354838707</v>
-      </c>
-      <c r="F7" s="95">
-        <v>65.47266280686857</v>
-      </c>
-      <c r="G7" s="95">
-        <v>84.03324265116818</v>
+      <c r="Y6" s="98" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="99">
+        <v>57.677419354838712</v>
+      </c>
+      <c r="C7" s="99">
+        <v>30.870967741935484</v>
+      </c>
+      <c r="D7" s="99">
+        <v>3675.2258064516127</v>
+      </c>
+      <c r="E7" s="99">
+        <v>688.61290322580646</v>
+      </c>
+      <c r="F7" s="100">
+        <v>65.212730667018491</v>
+      </c>
+      <c r="G7" s="100">
+        <v>84.219869076605278</v>
       </c>
       <c r="J7" s="32" t="s">
         <v>14</v>
@@ -1918,31 +1966,34 @@
       <c r="W7" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="X7" s="93" t="s">
+      <c r="X7" s="55" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="85">
-        <v>58.387096774193552</v>
-      </c>
-      <c r="C8" s="85">
-        <v>30.161290322580644</v>
-      </c>
-      <c r="D8" s="85">
-        <v>3643.8387096774195</v>
-      </c>
-      <c r="E8" s="85">
-        <v>720</v>
-      </c>
-      <c r="F8" s="29">
-        <v>65.966205960882803</v>
-      </c>
-      <c r="G8" s="29">
-        <v>83.5018913340908</v>
+      <c r="Y7" s="98" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="90">
+        <v>57.935483870967744</v>
+      </c>
+      <c r="C8" s="90">
+        <v>30.612903225806452</v>
+      </c>
+      <c r="D8" s="90">
+        <v>3667.0645161290322</v>
+      </c>
+      <c r="E8" s="90">
+        <v>696.77419354838707</v>
+      </c>
+      <c r="F8" s="56">
+        <v>65.47266280686857</v>
+      </c>
+      <c r="G8" s="56">
+        <v>84.03324265116818</v>
       </c>
       <c r="J8" s="32" t="s">
         <v>32</v>
@@ -1986,31 +2037,34 @@
       <c r="W8" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="X8" s="93" t="s">
+      <c r="X8" s="55" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="86">
-        <v>47</v>
-      </c>
-      <c r="C9" s="86">
-        <v>42</v>
-      </c>
-      <c r="D9" s="86">
-        <v>3749</v>
-      </c>
-      <c r="E9" s="86">
-        <v>614</v>
-      </c>
-      <c r="F9" s="3">
-        <v>53.88</v>
-      </c>
-      <c r="G9" s="3">
-        <v>85.96</v>
+      <c r="Y8" s="105" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="91">
+        <v>58.387096774193552</v>
+      </c>
+      <c r="C9" s="91">
+        <v>30.161290322580644</v>
+      </c>
+      <c r="D9" s="91">
+        <v>3643.8387096774195</v>
+      </c>
+      <c r="E9" s="91">
+        <v>720</v>
+      </c>
+      <c r="F9" s="29">
+        <v>65.966205960882803</v>
+      </c>
+      <c r="G9" s="29">
+        <v>83.5018913340908</v>
       </c>
       <c r="J9" s="32" t="s">
         <v>15</v>
@@ -2054,31 +2108,34 @@
       <c r="W9" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="X9" s="93" t="s">
+      <c r="X9" s="55" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="87">
-        <v>57.548387096774192</v>
-      </c>
-      <c r="C10" s="87">
-        <v>31</v>
-      </c>
-      <c r="D10" s="87">
-        <v>3690.9032258064517</v>
-      </c>
-      <c r="E10" s="87">
-        <v>672.93548387096769</v>
-      </c>
-      <c r="F10" s="10">
-        <v>64.890597828680242</v>
-      </c>
-      <c r="G10" s="10">
-        <v>84.580813641304928</v>
+      <c r="Y9" s="98" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="92">
+        <v>47</v>
+      </c>
+      <c r="C10" s="92">
+        <v>42</v>
+      </c>
+      <c r="D10" s="92">
+        <v>3749</v>
+      </c>
+      <c r="E10" s="92">
+        <v>614</v>
+      </c>
+      <c r="F10" s="3">
+        <v>53.88</v>
+      </c>
+      <c r="G10" s="3">
+        <v>85.96</v>
       </c>
       <c r="J10" s="32" t="s">
         <v>27</v>
@@ -2122,31 +2179,34 @@
       <c r="W10" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="X10" s="93" t="s">
+      <c r="X10" s="55" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="88">
-        <v>47.70967741935484</v>
-      </c>
-      <c r="C11" s="88">
-        <v>40.838709677419352</v>
-      </c>
-      <c r="D11" s="88">
-        <v>3722.5806451612902</v>
-      </c>
-      <c r="E11" s="88">
-        <v>641.25806451612902</v>
-      </c>
-      <c r="F11" s="20">
-        <v>54.925524644539941</v>
-      </c>
-      <c r="G11" s="20">
-        <v>85.316371139179736</v>
+      <c r="Y10" s="106" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="93">
+        <v>57.548387096774192</v>
+      </c>
+      <c r="C11" s="93">
+        <v>31</v>
+      </c>
+      <c r="D11" s="93">
+        <v>3690.9032258064517</v>
+      </c>
+      <c r="E11" s="93">
+        <v>672.93548387096769</v>
+      </c>
+      <c r="F11" s="10">
+        <v>64.890597828680242</v>
+      </c>
+      <c r="G11" s="10">
+        <v>84.580813641304928</v>
       </c>
       <c r="J11" s="32" t="s">
         <v>16</v>
@@ -2193,28 +2253,31 @@
       <c r="X11" s="30" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="89">
-        <v>47</v>
-      </c>
-      <c r="C12" s="89">
-        <v>42</v>
-      </c>
-      <c r="D12" s="89">
-        <v>3744</v>
-      </c>
-      <c r="E12" s="89">
-        <v>618</v>
-      </c>
-      <c r="F12" s="5">
-        <v>54.23</v>
-      </c>
-      <c r="G12" s="5">
-        <v>85.85</v>
+      <c r="Y11" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="94">
+        <v>47.70967741935484</v>
+      </c>
+      <c r="C12" s="94">
+        <v>40.838709677419352</v>
+      </c>
+      <c r="D12" s="94">
+        <v>3722.5806451612902</v>
+      </c>
+      <c r="E12" s="94">
+        <v>641.25806451612902</v>
+      </c>
+      <c r="F12" s="20">
+        <v>54.925524644539941</v>
+      </c>
+      <c r="G12" s="20">
+        <v>85.316371139179736</v>
       </c>
       <c r="J12" s="32" t="s">
         <v>42</v>
@@ -2261,28 +2324,31 @@
       <c r="X12" s="30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="90">
-        <v>46.258064516129032</v>
-      </c>
-      <c r="C13" s="90">
-        <v>42.29032258064516</v>
-      </c>
-      <c r="D13" s="90">
-        <v>3826.9677419354839</v>
-      </c>
-      <c r="E13" s="90">
-        <v>536.87096774193549</v>
-      </c>
-      <c r="F13" s="36">
-        <v>52.787579755345718</v>
-      </c>
-      <c r="G13" s="36">
-        <v>87.721533344561493</v>
+      <c r="Y12" s="30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="95">
+        <v>47</v>
+      </c>
+      <c r="C13" s="95">
+        <v>42</v>
+      </c>
+      <c r="D13" s="95">
+        <v>3744</v>
+      </c>
+      <c r="E13" s="95">
+        <v>618</v>
+      </c>
+      <c r="F13" s="5">
+        <v>54.23</v>
+      </c>
+      <c r="G13" s="5">
+        <v>85.85</v>
       </c>
       <c r="J13" s="32" t="s">
         <v>18</v>
@@ -2329,28 +2395,31 @@
       <c r="X13" s="30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="91">
-        <v>57.41935483870968</v>
-      </c>
-      <c r="C14" s="91">
-        <v>31.129032258064516</v>
-      </c>
-      <c r="D14" s="91">
-        <v>3692.0967741935483</v>
-      </c>
-      <c r="E14" s="91">
-        <v>671.74193548387098</v>
-      </c>
-      <c r="F14" s="39">
-        <v>64.817892699130013</v>
-      </c>
-      <c r="G14" s="39">
-        <v>84.607038002688725</v>
+      <c r="Y13" s="30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="96">
+        <v>46.258064516129032</v>
+      </c>
+      <c r="C14" s="96">
+        <v>42.29032258064516</v>
+      </c>
+      <c r="D14" s="96">
+        <v>3826.9677419354839</v>
+      </c>
+      <c r="E14" s="96">
+        <v>536.87096774193549</v>
+      </c>
+      <c r="F14" s="36">
+        <v>52.787579755345718</v>
+      </c>
+      <c r="G14" s="36">
+        <v>87.721533344561493</v>
       </c>
       <c r="J14" s="32" t="s">
         <v>19</v>
@@ -2385,8 +2454,32 @@
       <c r="X14" s="30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y14" s="30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="97">
+        <v>57.41935483870968</v>
+      </c>
+      <c r="C15" s="97">
+        <v>31.129032258064516</v>
+      </c>
+      <c r="D15" s="97">
+        <v>3692.0967741935483</v>
+      </c>
+      <c r="E15" s="97">
+        <v>671.74193548387098</v>
+      </c>
+      <c r="F15" s="39">
+        <v>64.817892699130013</v>
+      </c>
+      <c r="G15" s="39">
+        <v>84.607038002688725</v>
+      </c>
       <c r="J15" s="32" t="s">
         <v>43</v>
       </c>
@@ -2420,8 +2513,11 @@
       <c r="X15" s="30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y15" s="30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="J16" s="32" t="s">
         <v>44</v>
       </c>
@@ -2455,8 +2551,11 @@
       <c r="X16" s="30" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y16" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="J17" s="32" t="s">
         <v>21</v>
       </c>
@@ -2490,8 +2589,11 @@
       <c r="X17" s="30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y17" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="J18" s="32" t="s">
         <v>22</v>
       </c>
@@ -2525,8 +2627,11 @@
       <c r="X18" s="30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y18" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="J19" s="32" t="s">
         <v>23</v>
       </c>
@@ -2560,8 +2665,11 @@
       <c r="X19" s="30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y19" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="J20" s="32" t="s">
         <v>24</v>
       </c>
@@ -2583,21 +2691,24 @@
       <c r="P20" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y20" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="60"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="63"/>
       <c r="J21" s="32" t="s">
         <v>25</v>
       </c>
@@ -2620,20 +2731,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="57"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="60"/>
       <c r="J22" s="32" t="s">
         <v>28</v>
       </c>
@@ -2656,20 +2767,20 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="63"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="66"/>
       <c r="J23" s="32" t="s">
         <v>29</v>
       </c>
@@ -2692,20 +2803,20 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="72"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="75"/>
       <c r="J24" s="32" t="s">
         <v>30</v>
       </c>
@@ -2728,20 +2839,20 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="75"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="78"/>
       <c r="J25" s="32" t="s">
         <v>45</v>
       </c>
@@ -2764,20 +2875,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="69"/>
       <c r="J26" s="32" t="s">
         <v>26</v>
       </c>
@@ -2800,20 +2911,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="69"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="72"/>
       <c r="J27" s="32" t="s">
         <v>33</v>
       </c>
@@ -2836,20 +2947,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
       <c r="J28" s="43" t="s">
         <v>34</v>
       </c>
@@ -2872,97 +2983,112 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="77" t="s">
+      <c r="B29" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="77"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="76" t="s">
+      <c r="B30" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="79" t="s">
+      <c r="B31" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="97" t="s">
+      <c r="B32" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="97"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="83"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="92" t="s">
+      <c r="A33" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="96" t="s">
+      <c r="B33" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="96"/>
-      <c r="F33" s="96"/>
-      <c r="G33" s="96"/>
-      <c r="H33" s="96"/>
-      <c r="I33" s="96"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="84"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="101" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="102"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="102"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="102"/>
+      <c r="I34" s="103"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A34:I34"/>
+  <mergeCells count="15">
+    <mergeCell ref="A35:I35"/>
     <mergeCell ref="B22:I22"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B23:I23"/>
@@ -2976,6 +3102,7 @@
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B32:I32"/>
     <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B34:I34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Did some preliminary 2021 predictions with the updated data
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
+++ b/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C53441E-4B06-4606-9193-806497BFCD17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786F272B-3C83-4C10-ACC1-DF09D687C887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="71">
   <si>
     <t>Model</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>roundAbout</t>
+  </si>
+  <si>
+    <t>T7 v2 2021 Test</t>
   </si>
 </sst>
 </file>
@@ -895,7 +898,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -959,90 +962,6 @@
     <xf numFmtId="0" fontId="16" fillId="45" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="45" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1059,18 +978,105 @@
     <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="46" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="46" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="46" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1442,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V32" sqref="V32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1546,7 @@
       <c r="X1" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="Y1" s="104" t="s">
+      <c r="Y1" s="73" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1548,16 +1554,16 @@
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="85">
+      <c r="B2" s="57">
         <v>59</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="57">
         <v>30</v>
       </c>
-      <c r="D2" s="85">
+      <c r="D2" s="57">
         <v>3641</v>
       </c>
-      <c r="E2" s="85">
+      <c r="E2" s="57">
         <v>721</v>
       </c>
       <c r="F2" s="7">
@@ -1611,7 +1617,7 @@
       <c r="X2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="Y2" s="98" t="s">
+      <c r="Y2" s="70" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1619,16 +1625,16 @@
       <c r="A3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="86">
+      <c r="B3" s="58">
         <v>58.612903225806448</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="58">
         <v>29.93548387096774</v>
       </c>
-      <c r="D3" s="86">
+      <c r="D3" s="58">
         <v>3648.1290322580644</v>
       </c>
-      <c r="E3" s="86">
+      <c r="E3" s="58">
         <v>715.70967741935488</v>
       </c>
       <c r="F3" s="23">
@@ -1682,7 +1688,7 @@
       <c r="X3" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" s="98" t="s">
+      <c r="Y3" s="70" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1690,16 +1696,16 @@
       <c r="A4" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="87">
+      <c r="B4" s="59">
         <v>58.612903225806448</v>
       </c>
-      <c r="C4" s="87">
+      <c r="C4" s="59">
         <v>29.93548387096774</v>
       </c>
-      <c r="D4" s="87">
+      <c r="D4" s="59">
         <v>3651.2580645161293</v>
       </c>
-      <c r="E4" s="87">
+      <c r="E4" s="59">
         <v>712.58064516129036</v>
       </c>
       <c r="F4" s="42">
@@ -1753,7 +1759,7 @@
       <c r="X4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="98" t="s">
+      <c r="Y4" s="70" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1761,16 +1767,16 @@
       <c r="A5" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="88">
+      <c r="B5" s="60">
         <v>57.741935483870968</v>
       </c>
-      <c r="C5" s="88">
+      <c r="C5" s="60">
         <v>30.806451612903224</v>
       </c>
-      <c r="D5" s="88">
+      <c r="D5" s="60">
         <v>3671.0645161290322</v>
       </c>
-      <c r="E5" s="88">
+      <c r="E5" s="60">
         <v>692.77419354838707</v>
       </c>
       <c r="F5" s="46">
@@ -1824,7 +1830,7 @@
       <c r="X5" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="Y5" s="98" t="s">
+      <c r="Y5" s="70" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1832,16 +1838,16 @@
       <c r="A6" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="89">
+      <c r="B6" s="61">
         <v>57.548387096774192</v>
       </c>
-      <c r="C6" s="89">
+      <c r="C6" s="61">
         <v>31</v>
       </c>
-      <c r="D6" s="89">
+      <c r="D6" s="61">
         <v>3680.483870967742</v>
       </c>
-      <c r="E6" s="89">
+      <c r="E6" s="61">
         <v>683.35483870967744</v>
       </c>
       <c r="F6" s="53">
@@ -1898,30 +1904,30 @@
       <c r="X6" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="98" t="s">
+      <c r="Y6" s="70" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="99">
+      <c r="B7" s="71">
         <v>57.677419354838712</v>
       </c>
-      <c r="C7" s="99">
+      <c r="C7" s="71">
         <v>30.870967741935484</v>
       </c>
-      <c r="D7" s="99">
+      <c r="D7" s="71">
         <v>3675.2258064516127</v>
       </c>
-      <c r="E7" s="99">
+      <c r="E7" s="71">
         <v>688.61290322580646</v>
       </c>
-      <c r="F7" s="100">
+      <c r="F7" s="72">
         <v>65.212730667018491</v>
       </c>
-      <c r="G7" s="100">
+      <c r="G7" s="72">
         <v>84.219869076605278</v>
       </c>
       <c r="J7" s="32" t="s">
@@ -1969,7 +1975,7 @@
       <c r="X7" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="Y7" s="98" t="s">
+      <c r="Y7" s="70" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1977,16 +1983,16 @@
       <c r="A8" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="90">
+      <c r="B8" s="62">
         <v>57.935483870967744</v>
       </c>
-      <c r="C8" s="90">
+      <c r="C8" s="62">
         <v>30.612903225806452</v>
       </c>
-      <c r="D8" s="90">
+      <c r="D8" s="62">
         <v>3667.0645161290322</v>
       </c>
-      <c r="E8" s="90">
+      <c r="E8" s="62">
         <v>696.77419354838707</v>
       </c>
       <c r="F8" s="56">
@@ -2040,7 +2046,7 @@
       <c r="X8" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="Y8" s="105" t="s">
+      <c r="Y8" s="74" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2048,16 +2054,16 @@
       <c r="A9" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="91">
+      <c r="B9" s="63">
         <v>58.387096774193552</v>
       </c>
-      <c r="C9" s="91">
+      <c r="C9" s="63">
         <v>30.161290322580644</v>
       </c>
-      <c r="D9" s="91">
+      <c r="D9" s="63">
         <v>3643.8387096774195</v>
       </c>
-      <c r="E9" s="91">
+      <c r="E9" s="63">
         <v>720</v>
       </c>
       <c r="F9" s="29">
@@ -2111,7 +2117,7 @@
       <c r="X9" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="Y9" s="98" t="s">
+      <c r="Y9" s="70" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2119,16 +2125,16 @@
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="92">
+      <c r="B10" s="64">
         <v>47</v>
       </c>
-      <c r="C10" s="92">
+      <c r="C10" s="64">
         <v>42</v>
       </c>
-      <c r="D10" s="92">
+      <c r="D10" s="64">
         <v>3749</v>
       </c>
-      <c r="E10" s="92">
+      <c r="E10" s="64">
         <v>614</v>
       </c>
       <c r="F10" s="3">
@@ -2182,7 +2188,7 @@
       <c r="X10" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="Y10" s="106" t="s">
+      <c r="Y10" s="75" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2190,16 +2196,16 @@
       <c r="A11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="93">
+      <c r="B11" s="65">
         <v>57.548387096774192</v>
       </c>
-      <c r="C11" s="93">
+      <c r="C11" s="65">
         <v>31</v>
       </c>
-      <c r="D11" s="93">
+      <c r="D11" s="65">
         <v>3690.9032258064517</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E11" s="65">
         <v>672.93548387096769</v>
       </c>
       <c r="F11" s="10">
@@ -2261,16 +2267,16 @@
       <c r="A12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="94">
+      <c r="B12" s="66">
         <v>47.70967741935484</v>
       </c>
-      <c r="C12" s="94">
+      <c r="C12" s="66">
         <v>40.838709677419352</v>
       </c>
-      <c r="D12" s="94">
+      <c r="D12" s="66">
         <v>3722.5806451612902</v>
       </c>
-      <c r="E12" s="94">
+      <c r="E12" s="66">
         <v>641.25806451612902</v>
       </c>
       <c r="F12" s="20">
@@ -2332,16 +2338,16 @@
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="95">
+      <c r="B13" s="67">
         <v>47</v>
       </c>
-      <c r="C13" s="95">
+      <c r="C13" s="67">
         <v>42</v>
       </c>
-      <c r="D13" s="95">
+      <c r="D13" s="67">
         <v>3744</v>
       </c>
-      <c r="E13" s="95">
+      <c r="E13" s="67">
         <v>618</v>
       </c>
       <c r="F13" s="5">
@@ -2403,16 +2409,16 @@
       <c r="A14" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="96">
+      <c r="B14" s="68">
         <v>46.258064516129032</v>
       </c>
-      <c r="C14" s="96">
+      <c r="C14" s="68">
         <v>42.29032258064516</v>
       </c>
-      <c r="D14" s="96">
+      <c r="D14" s="68">
         <v>3826.9677419354839</v>
       </c>
-      <c r="E14" s="96">
+      <c r="E14" s="68">
         <v>536.87096774193549</v>
       </c>
       <c r="F14" s="36">
@@ -2462,16 +2468,16 @@
       <c r="A15" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="97">
+      <c r="B15" s="69">
         <v>57.41935483870968</v>
       </c>
-      <c r="C15" s="97">
+      <c r="C15" s="69">
         <v>31.129032258064516</v>
       </c>
-      <c r="D15" s="97">
+      <c r="D15" s="69">
         <v>3692.0967741935483</v>
       </c>
-      <c r="E15" s="97">
+      <c r="E15" s="69">
         <v>671.74193548387098</v>
       </c>
       <c r="F15" s="39">
@@ -2518,6 +2524,27 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="107" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="108">
+        <v>39.041666666666664</v>
+      </c>
+      <c r="C16" s="108">
+        <v>22.666666666666668</v>
+      </c>
+      <c r="D16" s="108">
+        <v>3708.0833333333335</v>
+      </c>
+      <c r="E16" s="108">
+        <v>676.58333333333337</v>
+      </c>
+      <c r="F16" s="109">
+        <v>63.960294341506433</v>
+      </c>
+      <c r="G16" s="109">
+        <v>84.575015461263874</v>
+      </c>
       <c r="J16" s="32" t="s">
         <v>44</v>
       </c>
@@ -2699,16 +2726,16 @@
       <c r="A21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="82"/>
       <c r="J21" s="32" t="s">
         <v>25</v>
       </c>
@@ -2735,16 +2762,16 @@
       <c r="A22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="60"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="79"/>
       <c r="J22" s="32" t="s">
         <v>28</v>
       </c>
@@ -2771,16 +2798,16 @@
       <c r="A23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="66"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="85"/>
       <c r="J23" s="32" t="s">
         <v>29</v>
       </c>
@@ -2807,16 +2834,16 @@
       <c r="A24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="75"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="93"/>
+      <c r="H24" s="93"/>
+      <c r="I24" s="94"/>
       <c r="J24" s="32" t="s">
         <v>30</v>
       </c>
@@ -2843,16 +2870,16 @@
       <c r="A25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="78"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="96"/>
+      <c r="I25" s="97"/>
       <c r="J25" s="32" t="s">
         <v>45</v>
       </c>
@@ -2879,16 +2906,16 @@
       <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="69"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="88"/>
       <c r="J26" s="32" t="s">
         <v>26</v>
       </c>
@@ -2915,16 +2942,16 @@
       <c r="A27" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="72"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="91"/>
       <c r="J27" s="32" t="s">
         <v>33</v>
       </c>
@@ -2951,16 +2978,16 @@
       <c r="A28" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="81"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
       <c r="J28" s="43" t="s">
         <v>34</v>
       </c>
@@ -2987,104 +3014,104 @@
       <c r="A29" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="80" t="s">
+      <c r="B29" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="80"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="99"/>
+      <c r="F29" s="99"/>
+      <c r="G29" s="99"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="99"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="79"/>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="79"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="98"/>
+      <c r="I30" s="98"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="82" t="s">
+      <c r="B31" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="82"/>
-      <c r="H31" s="82"/>
-      <c r="I31" s="82"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="101"/>
+      <c r="I31" s="101"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
+      <c r="C32" s="102"/>
+      <c r="D32" s="102"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="102"/>
+      <c r="G32" s="102"/>
+      <c r="H32" s="102"/>
+      <c r="I32" s="102"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="84" t="s">
+      <c r="B33" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="84"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="98" t="s">
+      <c r="A34" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="101" t="s">
+      <c r="B34" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="102"/>
-      <c r="D34" s="102"/>
-      <c r="E34" s="102"/>
-      <c r="F34" s="102"/>
-      <c r="G34" s="102"/>
-      <c r="H34" s="102"/>
-      <c r="I34" s="103"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="105"/>
+      <c r="E34" s="105"/>
+      <c r="F34" s="105"/>
+      <c r="G34" s="105"/>
+      <c r="H34" s="105"/>
+      <c r="I34" s="106"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Fetched missing June 2020 weather that was messing up our 2020 dataset
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
+++ b/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786F272B-3C83-4C10-ACC1-DF09D687C887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4A59DC-A9EE-4813-8594-3D94A396E8B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="70">
   <si>
     <t>Model</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>roundAbout</t>
-  </si>
-  <si>
-    <t>T7 v2 2021 Test</t>
   </si>
 </sst>
 </file>
@@ -981,102 +978,102 @@
     <xf numFmtId="0" fontId="16" fillId="46" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1449,7 +1446,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,27 +2521,13 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="107" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="108">
-        <v>39.041666666666664</v>
-      </c>
-      <c r="C16" s="108">
-        <v>22.666666666666668</v>
-      </c>
-      <c r="D16" s="108">
-        <v>3708.0833333333335</v>
-      </c>
-      <c r="E16" s="108">
-        <v>676.58333333333337</v>
-      </c>
-      <c r="F16" s="109">
-        <v>63.960294341506433</v>
-      </c>
-      <c r="G16" s="109">
-        <v>84.575015461263874</v>
-      </c>
+      <c r="A16" s="76"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
       <c r="J16" s="32" t="s">
         <v>44</v>
       </c>
@@ -2726,16 +2709,16 @@
       <c r="A21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="82"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="85"/>
       <c r="J21" s="32" t="s">
         <v>25</v>
       </c>
@@ -2762,16 +2745,16 @@
       <c r="A22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="79"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="82"/>
       <c r="J22" s="32" t="s">
         <v>28</v>
       </c>
@@ -2798,16 +2781,16 @@
       <c r="A23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="85"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="88"/>
       <c r="J23" s="32" t="s">
         <v>29</v>
       </c>
@@ -2834,16 +2817,16 @@
       <c r="A24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="92" t="s">
+      <c r="B24" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="93"/>
-      <c r="I24" s="94"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="96"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="97"/>
       <c r="J24" s="32" t="s">
         <v>30</v>
       </c>
@@ -2870,16 +2853,16 @@
       <c r="A25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="96"/>
-      <c r="I25" s="97"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="99"/>
+      <c r="G25" s="99"/>
+      <c r="H25" s="99"/>
+      <c r="I25" s="100"/>
       <c r="J25" s="32" t="s">
         <v>45</v>
       </c>
@@ -2906,16 +2889,16 @@
       <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="88"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="91"/>
       <c r="J26" s="32" t="s">
         <v>26</v>
       </c>
@@ -2942,16 +2925,16 @@
       <c r="A27" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="91"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="94"/>
       <c r="J27" s="32" t="s">
         <v>33</v>
       </c>
@@ -2978,16 +2961,16 @@
       <c r="A28" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="100" t="s">
+      <c r="B28" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="100"/>
-      <c r="I28" s="100"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="103"/>
       <c r="J28" s="43" t="s">
         <v>34</v>
       </c>
@@ -3014,104 +2997,104 @@
       <c r="A29" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="99" t="s">
+      <c r="B29" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
+      <c r="C29" s="102"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="98"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="98"/>
-      <c r="F30" s="98"/>
-      <c r="G30" s="98"/>
-      <c r="H30" s="98"/>
-      <c r="I30" s="98"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="101"/>
+      <c r="H30" s="101"/>
+      <c r="I30" s="101"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="101"/>
-      <c r="I31" s="101"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="104"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="102" t="s">
+      <c r="B32" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="102"/>
-      <c r="D32" s="102"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="102"/>
-      <c r="H32" s="102"/>
-      <c r="I32" s="102"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="105"/>
+      <c r="I32" s="105"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="103" t="s">
+      <c r="B33" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="103"/>
-      <c r="D33" s="103"/>
-      <c r="E33" s="103"/>
-      <c r="F33" s="103"/>
-      <c r="G33" s="103"/>
-      <c r="H33" s="103"/>
-      <c r="I33" s="103"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="106"/>
+      <c r="I33" s="106"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="104" t="s">
+      <c r="B34" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="105"/>
-      <c r="G34" s="105"/>
-      <c r="H34" s="105"/>
-      <c r="I34" s="106"/>
+      <c r="C34" s="108"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="108"/>
+      <c r="G34" s="108"/>
+      <c r="H34" s="108"/>
+      <c r="I34" s="109"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="76"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Did first round of predictions for 2021. Also, updated our list of accidents retrieved via email code.
</commit_message>
<xml_diff>
--- a/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
+++ b/Main Dir/Logistic Regression Tests/LogReg Variable Significance Tests (OLS vs T1 Alt vs Thesis).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Main Dir\Logistic Regression Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4A59DC-A9EE-4813-8594-3D94A396E8B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B7052C-6416-44E9-A684-93297DA32E52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="71">
   <si>
     <t>Model</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>roundAbout</t>
+  </si>
+  <si>
+    <t>2021 Prediction</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1449,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,13 +2524,27 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
+      <c r="A16" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="77">
+        <v>37.548387096774192</v>
+      </c>
+      <c r="C16" s="77">
+        <v>25.06451612903226</v>
+      </c>
+      <c r="D16" s="77">
+        <v>3769.1290322580644</v>
+      </c>
+      <c r="E16" s="77">
+        <v>620.64516129032256</v>
+      </c>
+      <c r="F16" s="78">
+        <v>60.384969394379581</v>
+      </c>
+      <c r="G16" s="78">
+        <v>85.865833847042154</v>
+      </c>
       <c r="J16" s="32" t="s">
         <v>44</v>
       </c>

</xml_diff>